<commit_message>
Add compressed type of report
</commit_message>
<xml_diff>
--- a/FeedbackSIUT/static/app/files/feedback_report_example.xlsx
+++ b/FeedbackSIUT/static/app/files/feedback_report_example.xlsx
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>________________________</t>
-  </si>
-  <si>
-    <t>Head of the Department</t>
   </si>
   <si>
     <t xml:space="preserve">      Academic Staff Evaluation</t>
@@ -73,10 +70,13 @@
     </r>
   </si>
   <si>
-    <t>Sayfullayev A.I.</t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Vice-Rector (Academics)</t>
+  </si>
+  <si>
+    <t>Communication and Leadership Skills (CLS)</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -162,15 +162,6 @@
         <color theme="4" tint="-0.499984740745262"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -199,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -225,44 +216,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="20"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="25"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="12"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="21"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="20"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="25"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="12"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -294,13 +282,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>578733</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>253196</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289366</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -323,7 +311,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1000727" y="-1000727"/>
+          <a:off x="1000727" y="-1000726"/>
           <a:ext cx="7511487" cy="9512942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -336,15 +324,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>434570</xdr:colOff>
+      <xdr:colOff>205487</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>24130</xdr:rowOff>
+      <xdr:rowOff>48244</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1114310</xdr:colOff>
+      <xdr:colOff>885227</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>186374</xdr:rowOff>
+      <xdr:rowOff>210488</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -367,7 +355,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4413367" y="277326"/>
+          <a:off x="4425424" y="301440"/>
           <a:ext cx="679740" cy="1066516"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -669,16 +657,16 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="5.140625" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
@@ -698,43 +686,43 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="25"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
     </row>
@@ -742,9 +730,9 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
     </row>
@@ -761,11 +749,11 @@
     <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="C8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
@@ -773,9 +761,9 @@
     <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
@@ -783,11 +771,11 @@
     <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="C10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -802,115 +790,117 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+    <row r="13" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="7"/>
       <c r="G13" s="5"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="16"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="11"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="11"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="11"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="11"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="11"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="11"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="11"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -920,21 +910,19 @@
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="11"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="24" t="s">
         <v>6</v>
       </c>
+      <c r="E24" s="24"/>
       <c r="F24" s="11"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -943,26 +931,28 @@
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="E25" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="D25" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="23"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C8:E9"/>
     <mergeCell ref="A3:C5"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="D2:F6"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.23622047244094491" top="0.11811023622047245" bottom="0.11811023622047245" header="0.31496062992125984" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>